<commit_message>
Corrections in Correlation analysis
</commit_message>
<xml_diff>
--- a/correlations/Correlations.xlsx
+++ b/correlations/Correlations.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21823"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="138" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{9D3B3486-00E5-4709-BC7A-F5FF98B365BE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80A4ACBC-E237-49A4-9434-B51B3349A87A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,13 +210,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -229,9 +232,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -551,7 +551,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,37 +568,37 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="3"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="10" t="s">
         <v>0</v>
       </c>
     </row>
@@ -607,8 +607,8 @@
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <f>111/296</f>
-        <v>0.375</v>
+        <f>M2/296</f>
+        <v>0.39527027027027029</v>
       </c>
       <c r="C2" s="1">
         <f>_xlfn.RANK.AVG(B2, $B$2:$B$6,0)</f>
@@ -635,15 +635,15 @@
         <f>_xlfn.RANK.AVG(H2, $H$2:$H$6,0)</f>
         <v>2</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="9">
+      <c r="K2" s="12"/>
+      <c r="L2" s="7">
         <v>16</v>
       </c>
       <c r="M2" s="1">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -651,8 +651,8 @@
         <v>12</v>
       </c>
       <c r="B3" s="1">
-        <f>47/66</f>
-        <v>0.71212121212121215</v>
+        <f>M3/66</f>
+        <v>0.75757575757575757</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C6" si="0">_xlfn.RANK.AVG(B3, $B$2:$B$6,0)</f>
@@ -681,14 +681,14 @@
       </c>
       <c r="J3" s="5">
         <f>CORREL(B2:B6, D2:D6)</f>
-        <v>0.35125097035306047</v>
+        <v>0.35358660720286889</v>
       </c>
       <c r="K3" s="6">
         <f>CORREL(C2:C6, E2:E6)</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="M3" s="1">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -696,8 +696,8 @@
         <v>13</v>
       </c>
       <c r="B4" s="1">
-        <f>16/126</f>
-        <v>0.12698412698412698</v>
+        <f>M4/127</f>
+        <v>0.13385826771653545</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
@@ -724,15 +724,15 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="9">
+      <c r="K4" s="14"/>
+      <c r="L4" s="7">
         <v>26</v>
       </c>
       <c r="M4" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -740,7 +740,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="1">
-        <f>49/297</f>
+        <f>M5/297</f>
         <v>0.16498316498316498</v>
       </c>
       <c r="C5" s="1">
@@ -770,7 +770,7 @@
       </c>
       <c r="J5" s="5">
         <f>CORREL(B2:B6, F2:F6)</f>
-        <v>0.35629544338001212</v>
+        <v>0.35823386968482035</v>
       </c>
       <c r="K5" s="6">
         <f>CORREL(C2:C6, G2:G6)</f>
@@ -785,7 +785,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1">
-        <f>111/38</f>
+        <f>M6/38</f>
         <v>2.9210526315789473</v>
       </c>
       <c r="C6" s="1">
@@ -813,11 +813,11 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="9">
+      <c r="K6" s="14"/>
+      <c r="L6" s="7">
         <v>56</v>
       </c>
       <c r="M6" s="1">
@@ -827,7 +827,7 @@
     <row r="7" spans="1:13">
       <c r="J7" s="5">
         <f>CORREL(B2:B6, H2:H6)</f>
-        <v>-0.71170347480841645</v>
+        <v>-0.71743128921760824</v>
       </c>
       <c r="K7" s="1">
         <f>CORREL(C2:C6, I2:I6)</f>

</xml_diff>